<commit_message>
Add to new columns app description, image, and links.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-mega-course\portfolio-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3A1018-3CFF-44A4-A4AB-755994F8FDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA49D7EA-68BC-4242-82EE-5A9FB766B56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5685" yWindow="1710" windowWidth="21600" windowHeight="11475" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>ToDo App</t>
   </si>
   <si>
@@ -102,6 +96,12 @@
   </si>
   <si>
     <t>Placeholder2</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Image</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,80 +535,80 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new application to programs.xlsx.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-mega-course\portfolio-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA49D7EA-68BC-4242-82EE-5A9FB766B56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A510D85-97F9-4566-BEAA-622C4581BE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5685" yWindow="1710" windowWidth="21600" windowHeight="11475" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
+    <workbookView xWindow="6255" yWindow="3675" windowWidth="21600" windowHeight="11475" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Python Programs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Title</t>
   </si>
@@ -92,9 +92,6 @@
     <t>5.png</t>
   </si>
   <si>
-    <t>Placeholder1</t>
-  </si>
-  <si>
     <t>Placeholder2</t>
   </si>
   <si>
@@ -102,6 +99,15 @@
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>Convert Table to Campaign Logger</t>
+  </si>
+  <si>
+    <t>This application allows the user to choose a csv file or an Excel workbook, the desired table or spreadsheet in the workbook, a destination folder, and the name of the textfile that will contain the converted table. This saves a lot of time for GMs who use a combination of spreadsheets and Campaign Logger reports.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/convert-table-to-cl-md</t>
   </si>
 </sst>
 </file>
@@ -185,8 +191,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -194,6 +198,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -503,7 +513,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -517,38 +527,38 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="63.42578125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="55.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="55.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -556,13 +566,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -570,41 +580,41 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -616,8 +626,9 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{979EE87F-DBC9-41F2-B27A-DF33CF8936A5}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{1AA70311-BC82-4672-B718-EE6EEFA30950}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{990FB6C7-A6E4-4582-AF02-F867B65C49B0}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{0103464B-0AAD-48F9-A055-0AC2B21ECB0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId4"/>
+  <picture r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add six additional applications to programs.xlsx.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-mega-course\portfolio-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A510D85-97F9-4566-BEAA-622C4581BE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181F3EC-9E26-4DD7-994C-6406172FD6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="3675" windowWidth="21600" windowHeight="11475" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
+    <workbookView xWindow="-20640" yWindow="5070" windowWidth="19740" windowHeight="10500" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Python Programs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Title</t>
   </si>
@@ -108,6 +108,51 @@
   </si>
   <si>
     <t>https://github.com/valenpendragon/convert-table-to-cl-md</t>
+  </si>
+  <si>
+    <t>History Skeleton Generator</t>
+  </si>
+  <si>
+    <t>This application is writen using Jupyter Notebook. Inside the notebook are the instructions for creating a Timeline workbook for the program to use to create an output workbook containing rough timelines for nations and factions in a fictional universe.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/history-skeleton-generator</t>
+  </si>
+  <si>
+    <t>Web Weather API</t>
+  </si>
+  <si>
+    <t>This application is a Flask website that provides climate data to the user using a URL API. Instructions for using the API are on the site's homepage.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/web-weather-api</t>
+  </si>
+  <si>
+    <t>NASA's Astronony Web Page</t>
+  </si>
+  <si>
+    <t>This is a simple Streamlit App that displays NASA's Astronomy Picture of the Day, including the Copyright information when it exists.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/apod-web-page</t>
+  </si>
+  <si>
+    <t>News API Email</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/news-api-email</t>
+  </si>
+  <si>
+    <t>This application gathers daily news on a specified topic and emails the article links to the User. It serves more to demonstrate how to add this functionality to a web site.</t>
+  </si>
+  <si>
+    <t>Spreadsheet to PDF Invoice generator</t>
+  </si>
+  <si>
+    <t>This is a backend application that takes spreadsheet invoices generated from another part of an application and turns them into PDF Invoices that can be emailed to customers.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/PDF-invoices</t>
   </si>
 </sst>
 </file>
@@ -521,13 +566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FA3EDD-6D5D-4A55-A59F-85514ADFBD12}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,17 +652,101 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -627,8 +756,13 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{1AA70311-BC82-4672-B718-EE6EEFA30950}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{990FB6C7-A6E4-4582-AF02-F867B65C49B0}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{0103464B-0AAD-48F9-A055-0AC2B21ECB0B}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{904B9E7B-45F8-4793-9E73-E7A85706E9F0}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{D62E6C05-C608-4C58-A7AD-8DE5D7575AB8}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{41528A17-1919-43EB-8F69-8FC124A515B0}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{EFA3C3A0-9718-440A-A76D-2F4C491D6C3B}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{ADF68116-6324-48A3-BD4E-F5AB923608BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId5"/>
+  <picture r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add two additional applications to programs.xlsx.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-mega-course\portfolio-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181F3EC-9E26-4DD7-994C-6406172FD6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8086CACE-62D7-484B-9203-024E8326586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20640" yWindow="5070" windowWidth="19740" windowHeight="10500" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
+    <workbookView xWindow="-20400" yWindow="5070" windowWidth="19740" windowHeight="10500" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Python Programs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>Title</t>
   </si>
@@ -153,6 +153,24 @@
   </si>
   <si>
     <t>https://github.com/valenpendragon/PDF-invoices</t>
+  </si>
+  <si>
+    <t>Happiness Analysis</t>
+  </si>
+  <si>
+    <t>Several factors, both economic and social, increase the happiness of populations in countries. The study data gathered for several contries is part of this application. The streamlit application allows the user to plot graphs of these factors and overall happiness.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/happiness-web-app</t>
+  </si>
+  <si>
+    <t>Weather Forecast Web App</t>
+  </si>
+  <si>
+    <t>This streamlit appliction gathers up to 5 days of forecast sky conditions and temperature data for a city they wish to view.</t>
+  </si>
+  <si>
+    <t>https://github.com/valenpendragon/weather-forecast-web-app</t>
   </si>
 </sst>
 </file>
@@ -566,13 +584,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FA3EDD-6D5D-4A55-A59F-85514ADFBD12}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,31 +740,45 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -761,8 +793,10 @@
     <hyperlink ref="C8" r:id="rId7" xr:uid="{41528A17-1919-43EB-8F69-8FC124A515B0}"/>
     <hyperlink ref="C9" r:id="rId8" xr:uid="{EFA3C3A0-9718-440A-A76D-2F4C491D6C3B}"/>
     <hyperlink ref="C10" r:id="rId9" xr:uid="{ADF68116-6324-48A3-BD4E-F5AB923608BC}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{EB475308-6E8C-4024-BB40-EB1939A63EC0}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{89B39863-2DED-4993-B80A-BE4501656562}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId10"/>
+  <picture r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove one application from programs.xlsx.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\valen\Documents\Valen\python\python-mega-course\portfolio-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8086CACE-62D7-484B-9203-024E8326586B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFD283E-66D0-4E2C-906F-AEE8765DAC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20400" yWindow="5070" windowWidth="19740" windowHeight="10500" xr2:uid="{9E0813F6-ED6A-45E5-954F-6101CCD1BF4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Title</t>
   </si>
@@ -135,15 +135,6 @@
   </si>
   <si>
     <t>https://github.com/valenpendragon/apod-web-page</t>
-  </si>
-  <si>
-    <t>News API Email</t>
-  </si>
-  <si>
-    <t>https://github.com/valenpendragon/news-api-email</t>
-  </si>
-  <si>
-    <t>This application gathers daily news on a specified topic and emails the article links to the User. It serves more to demonstrate how to add this functionality to a web site.</t>
   </si>
   <si>
     <t>Spreadsheet to PDF Invoice generator</t>
@@ -584,13 +575,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FA3EDD-6D5D-4A55-A59F-85514ADFBD12}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,16 +708,16 @@
         <v>33</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
@@ -740,7 +731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>39</v>
       </c>
@@ -754,31 +745,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -791,12 +768,11 @@
     <hyperlink ref="C6" r:id="rId5" xr:uid="{904B9E7B-45F8-4793-9E73-E7A85706E9F0}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{D62E6C05-C608-4C58-A7AD-8DE5D7575AB8}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{41528A17-1919-43EB-8F69-8FC124A515B0}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{EFA3C3A0-9718-440A-A76D-2F4C491D6C3B}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{ADF68116-6324-48A3-BD4E-F5AB923608BC}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{EB475308-6E8C-4024-BB40-EB1939A63EC0}"/>
-    <hyperlink ref="C12" r:id="rId11" xr:uid="{89B39863-2DED-4993-B80A-BE4501656562}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{ADF68116-6324-48A3-BD4E-F5AB923608BC}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{EB475308-6E8C-4024-BB40-EB1939A63EC0}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{89B39863-2DED-4993-B80A-BE4501656562}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId12"/>
+  <picture r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>